<commit_message>
Remove Goal Bias from output parameter file when GoalType is 0
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/TransferFile.xlsx
+++ b/doc/Manual/Batchmode/TransferFile.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RangeShifter2_SCFP_files\Distribution\RS_v2.0_209999\Batch_documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RangeShifter2\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FECCD2-B38C-48BD-BA1C-3166D5BDAA25}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="20730" windowHeight="9780"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description Kernels" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="167">
   <si>
     <t>NOTES</t>
   </si>
@@ -825,11 +826,14 @@
   <si>
     <t>Per-step mortality type: 0 = constant, 1 = habitat-dependent</t>
   </si>
+  <si>
+    <t>Must be &gt;= 1.0; applies only when GoalType = 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1140,6 +1144,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1158,9 +1165,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1257,6 +1261,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1292,6 +1313,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1467,7 +1505,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1477,16 +1515,16 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.5703125" style="38" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="28"/>
+    <col min="4" max="4" width="55.5546875" style="38" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>46</v>
       </c>
@@ -1500,7 +1538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>22</v>
       </c>
@@ -1514,7 +1552,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
@@ -1528,7 +1566,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>24</v>
       </c>
@@ -1540,7 +1578,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -1552,7 +1590,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
@@ -1564,7 +1602,7 @@
       </c>
       <c r="D6" s="35"/>
     </row>
-    <row r="7" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1578,7 +1616,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1590,7 +1628,7 @@
       </c>
       <c r="D8" s="35"/>
     </row>
-    <row r="9" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1602,7 +1640,7 @@
       </c>
       <c r="D9" s="35"/>
     </row>
-    <row r="10" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>26</v>
       </c>
@@ -1612,11 +1650,11 @@
       <c r="C10" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="62" t="s">
+      <c r="D10" s="65" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>27</v>
       </c>
@@ -1626,9 +1664,9 @@
       <c r="C11" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="63"/>
-    </row>
-    <row r="12" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="66"/>
+    </row>
+    <row r="12" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>28</v>
       </c>
@@ -1640,7 +1678,7 @@
       </c>
       <c r="D12" s="32"/>
     </row>
-    <row r="13" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="51" t="s">
         <v>102</v>
       </c>
@@ -1654,7 +1692,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="51" t="s">
         <v>103</v>
       </c>
@@ -1668,7 +1706,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="51" t="s">
         <v>104</v>
       </c>
@@ -1682,7 +1720,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="51" t="s">
         <v>105</v>
       </c>
@@ -1696,7 +1734,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="51" t="s">
         <v>106</v>
       </c>
@@ -1710,7 +1748,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="51" t="s">
         <v>107</v>
       </c>
@@ -1724,7 +1762,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="46" t="s">
         <v>109</v>
       </c>
@@ -1738,7 +1776,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="46" t="s">
         <v>110</v>
       </c>
@@ -1752,7 +1790,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="46" t="s">
         <v>108</v>
       </c>
@@ -1766,7 +1804,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -1778,7 +1816,7 @@
       </c>
       <c r="D22" s="35"/>
     </row>
-    <row r="23" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -1790,7 +1828,7 @@
       </c>
       <c r="D23" s="36"/>
     </row>
-    <row r="24" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -1802,218 +1840,218 @@
       </c>
       <c r="D24" s="36"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="26"/>
       <c r="B25" s="26"/>
       <c r="C25" s="27"/>
       <c r="D25" s="37"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="26"/>
       <c r="B26" s="26"/>
       <c r="C26" s="29"/>
       <c r="D26" s="37"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="26"/>
       <c r="B27" s="26"/>
       <c r="C27" s="29"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="26"/>
       <c r="B28" s="26"/>
       <c r="C28" s="29"/>
       <c r="D28" s="37"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="26"/>
       <c r="B29" s="26"/>
       <c r="C29" s="29"/>
       <c r="D29" s="37"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="26"/>
       <c r="B30" s="26"/>
       <c r="C30" s="29"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="26"/>
       <c r="B31" s="26"/>
       <c r="C31" s="29"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="26"/>
       <c r="B32" s="26"/>
       <c r="C32" s="29"/>
       <c r="D32" s="37"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="26"/>
       <c r="B33" s="26"/>
       <c r="C33" s="29"/>
       <c r="D33" s="37"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="26"/>
       <c r="B34" s="26"/>
       <c r="C34" s="29"/>
       <c r="D34" s="37"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="26"/>
       <c r="B35" s="26"/>
       <c r="C35" s="29"/>
       <c r="D35" s="37"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C36" s="29"/>
       <c r="D36" s="37"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C37" s="29"/>
       <c r="D37" s="37"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C38" s="29"/>
       <c r="D38" s="37"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C39" s="29"/>
       <c r="D39" s="37"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C40" s="29"/>
       <c r="D40" s="37"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C41" s="29"/>
       <c r="D41" s="37"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C42" s="29"/>
       <c r="D42" s="37"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C43" s="29"/>
       <c r="D43" s="37"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C44" s="29"/>
       <c r="D44" s="37"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C45" s="29"/>
       <c r="D45" s="37"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C46" s="29"/>
       <c r="D46" s="37"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C47" s="29"/>
       <c r="D47" s="37"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C48" s="29"/>
       <c r="D48" s="37"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49" s="29"/>
       <c r="D49" s="37"/>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50" s="29"/>
       <c r="D50" s="37"/>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C51" s="29"/>
       <c r="D51" s="37"/>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C52" s="29"/>
       <c r="D52" s="37"/>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C53" s="29"/>
       <c r="D53" s="37"/>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C54" s="29"/>
       <c r="D54" s="37"/>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C55" s="29"/>
       <c r="D55" s="37"/>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C56" s="29"/>
       <c r="D56" s="37"/>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C57" s="29"/>
       <c r="D57" s="37"/>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C58" s="29"/>
       <c r="D58" s="37"/>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C59" s="29"/>
       <c r="D59" s="37"/>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C60" s="29"/>
       <c r="D60" s="37"/>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C61" s="29"/>
       <c r="D61" s="37"/>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C62" s="29"/>
       <c r="D62" s="37"/>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C63" s="29"/>
       <c r="D63" s="37"/>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C64" s="29"/>
       <c r="D64" s="37"/>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C65" s="29"/>
       <c r="D65" s="37"/>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C66" s="29"/>
       <c r="D66" s="37"/>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C67" s="29"/>
       <c r="D67" s="37"/>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C68" s="29"/>
       <c r="D68" s="37"/>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C69" s="29"/>
       <c r="D69" s="37"/>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C70" s="29"/>
       <c r="D70" s="37"/>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C71" s="29"/>
       <c r="D71" s="37"/>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C72" s="29"/>
       <c r="D72" s="37"/>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C73" s="29"/>
       <c r="D73" s="37"/>
     </row>
@@ -2027,7 +2065,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2037,15 +2075,15 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="83" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>46</v>
       </c>
@@ -2059,7 +2097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>22</v>
       </c>
@@ -2073,7 +2111,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2085,7 +2123,7 @@
       </c>
       <c r="D3" s="24"/>
     </row>
-    <row r="4" spans="1:4" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>16</v>
       </c>
@@ -2099,7 +2137,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>44</v>
       </c>
@@ -2113,7 +2151,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="51" t="s">
         <v>117</v>
       </c>
@@ -2127,7 +2165,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="51" t="s">
         <v>118</v>
       </c>
@@ -2141,7 +2179,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="51" t="s">
         <v>119</v>
       </c>
@@ -2155,7 +2193,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="51" t="s">
         <v>120</v>
       </c>
@@ -2169,7 +2207,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="46" t="s">
         <v>121</v>
       </c>
@@ -2183,7 +2221,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="46" t="s">
         <v>124</v>
       </c>
@@ -2197,7 +2235,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="56" t="s">
         <v>127</v>
       </c>
@@ -2209,7 +2247,7 @@
       </c>
       <c r="D12" s="59"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2221,7 +2259,7 @@
       </c>
       <c r="D13" s="24"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2235,7 +2273,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>65</v>
       </c>
@@ -2245,11 +2283,11 @@
       <c r="C15" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="64" t="s">
+      <c r="D15" s="67" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>64</v>
       </c>
@@ -2259,277 +2297,277 @@
       <c r="C16" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="65"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="68"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17" s="2"/>
       <c r="D17" s="17"/>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18" s="2"/>
       <c r="D18" s="17"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" s="2"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20" s="2"/>
       <c r="D20" s="17"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21" s="2"/>
       <c r="D21" s="17"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" s="2"/>
       <c r="D22" s="17"/>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C23" s="2"/>
       <c r="D23" s="17"/>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C24" s="2"/>
       <c r="D24" s="17"/>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C25" s="2"/>
       <c r="D25" s="17"/>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C26" s="2"/>
       <c r="D26" s="17"/>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C27" s="2"/>
       <c r="D27" s="17"/>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C28" s="2"/>
       <c r="D28" s="17"/>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C29" s="2"/>
       <c r="D29" s="17"/>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C30" s="2"/>
       <c r="D30" s="17"/>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C31" s="2"/>
       <c r="D31" s="17"/>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C32" s="2"/>
       <c r="D32" s="17"/>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C33" s="2"/>
       <c r="D33" s="17"/>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C34" s="2"/>
       <c r="D34" s="17"/>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C35" s="2"/>
       <c r="D35" s="17"/>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C36" s="2"/>
       <c r="D36" s="17"/>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C37" s="2"/>
       <c r="D37" s="17"/>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C38" s="2"/>
       <c r="D38" s="17"/>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C39" s="2"/>
       <c r="D39" s="17"/>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C40" s="2"/>
       <c r="D40" s="17"/>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C41" s="2"/>
       <c r="D41" s="17"/>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C42" s="2"/>
       <c r="D42" s="17"/>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C43" s="2"/>
       <c r="D43" s="17"/>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C44" s="2"/>
       <c r="D44" s="17"/>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C45" s="2"/>
       <c r="D45" s="17"/>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C46" s="2"/>
       <c r="D46" s="17"/>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C47" s="2"/>
       <c r="D47" s="17"/>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C48" s="2"/>
       <c r="D48" s="17"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49" s="2"/>
       <c r="D49" s="17"/>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50" s="2"/>
       <c r="D50" s="17"/>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C51" s="2"/>
       <c r="D51" s="17"/>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C52" s="2"/>
       <c r="D52" s="17"/>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C53" s="2"/>
       <c r="D53" s="17"/>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C54" s="2"/>
       <c r="D54" s="17"/>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C55" s="2"/>
       <c r="D55" s="17"/>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C56" s="2"/>
       <c r="D56" s="17"/>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C57" s="2"/>
       <c r="D57" s="17"/>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C58" s="2"/>
       <c r="D58" s="17"/>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C59" s="2"/>
       <c r="D59" s="17"/>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C60" s="2"/>
       <c r="D60" s="17"/>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C61" s="2"/>
       <c r="D61" s="17"/>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C62" s="2"/>
       <c r="D62" s="17"/>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C63" s="2"/>
       <c r="D63" s="17"/>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C64" s="2"/>
       <c r="D64" s="17"/>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C65" s="2"/>
       <c r="D65" s="17"/>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C66" s="2"/>
       <c r="D66" s="17"/>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C67" s="2"/>
       <c r="D67" s="17"/>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C68" s="2"/>
       <c r="D68" s="17"/>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C69" s="2"/>
       <c r="D69" s="17"/>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C70" s="2"/>
       <c r="D70" s="17"/>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C71" s="2"/>
       <c r="D71" s="17"/>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C72" s="2"/>
       <c r="D72" s="17"/>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C73" s="2"/>
       <c r="D73" s="17"/>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C74" s="2"/>
       <c r="D74" s="17"/>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C75" s="2"/>
       <c r="D75" s="17"/>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C76" s="2"/>
       <c r="D76" s="17"/>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C77" s="2"/>
       <c r="D77" s="17"/>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C78" s="2"/>
       <c r="D78" s="17"/>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C79" s="2"/>
       <c r="D79" s="17"/>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C80" s="2"/>
       <c r="D80" s="17"/>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C81" s="2"/>
       <c r="D81" s="17"/>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C82" s="2"/>
       <c r="D82" s="17"/>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C83" s="2"/>
       <c r="D83" s="17"/>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C84" s="2"/>
       <c r="D84" s="17"/>
     </row>
@@ -2542,7 +2580,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2552,26 +2590,26 @@
       <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="53" t="s">
         <v>22</v>
       </c>
@@ -2621,7 +2659,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2671,7 +2709,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2721,7 +2759,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2771,7 +2809,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2827,7 +2865,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2837,22 +2875,22 @@
       <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="28" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="53" t="s">
         <v>22</v>
       </c>
@@ -2893,7 +2931,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2934,7 +2972,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2981,7 +3019,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2991,34 +3029,34 @@
       <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -3089,7 +3127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="39">
         <v>1</v>
       </c>
@@ -3160,7 +3198,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3231,7 +3269,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="39">
         <v>3</v>
       </c>
@@ -3302,7 +3340,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3373,7 +3411,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="39">
         <v>5</v>
       </c>
@@ -3444,7 +3482,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3515,7 +3553,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="39">
         <v>7</v>
       </c>
@@ -3586,7 +3624,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3657,7 +3695,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="39">
         <v>9</v>
       </c>
@@ -3728,7 +3766,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3799,7 +3837,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="39">
         <v>11</v>
       </c>
@@ -3870,7 +3908,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3947,7 +3985,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3957,34 +3995,34 @@
       <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -4055,7 +4093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="39">
         <v>1</v>
       </c>
@@ -4126,7 +4164,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4197,7 +4235,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="39">
         <v>3</v>
       </c>
@@ -4268,7 +4306,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4339,7 +4377,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="39">
         <v>5</v>
       </c>
@@ -4410,7 +4448,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4481,7 +4519,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="39">
         <v>7</v>
       </c>
@@ -4552,7 +4590,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4623,7 +4661,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="39">
         <v>9</v>
       </c>
@@ -4694,7 +4732,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4765,7 +4803,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="39">
         <v>11</v>
       </c>
@@ -4836,7 +4874,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4907,7 +4945,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="39">
         <v>13</v>
       </c>
@@ -4978,7 +5016,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="39">
         <v>13</v>
       </c>
@@ -5049,7 +5087,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -5120,7 +5158,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>14</v>
       </c>
@@ -5191,7 +5229,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="39">
         <v>15</v>
       </c>
@@ -5262,7 +5300,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="39">
         <v>15</v>
       </c>
@@ -5333,7 +5371,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>16</v>
       </c>
@@ -5404,7 +5442,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>16</v>
       </c>
@@ -5475,7 +5513,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="39">
         <v>17</v>
       </c>
@@ -5546,7 +5584,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="39">
         <v>17</v>
       </c>
@@ -5617,7 +5655,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>18</v>
       </c>
@@ -5688,7 +5726,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>18</v>
       </c>
@@ -5759,7 +5797,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="39">
         <v>19</v>
       </c>
@@ -5830,7 +5868,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="39">
         <v>19</v>
       </c>
@@ -5901,7 +5939,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>20</v>
       </c>
@@ -5972,7 +6010,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>20</v>
       </c>
@@ -6043,7 +6081,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="39">
         <v>21</v>
       </c>
@@ -6114,7 +6152,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="39">
         <v>21</v>
       </c>
@@ -6185,7 +6223,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>22</v>
       </c>
@@ -6256,7 +6294,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>22</v>
       </c>
@@ -6327,7 +6365,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" s="39">
         <v>23</v>
       </c>
@@ -6398,7 +6436,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" s="39">
         <v>23</v>
       </c>
@@ -6469,7 +6507,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>24</v>
       </c>
@@ -6540,7 +6578,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>24</v>
       </c>
@@ -6617,7 +6655,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -6628,34 +6666,34 @@
       <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -6726,7 +6764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="39">
         <v>1</v>
       </c>
@@ -6797,7 +6835,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6868,7 +6906,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="39">
         <v>3</v>
       </c>
@@ -6939,7 +6977,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7010,7 +7048,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="39">
         <v>5</v>
       </c>
@@ -7081,7 +7119,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="39">
         <v>5</v>
       </c>
@@ -7152,7 +7190,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="39">
         <v>5</v>
       </c>
@@ -7223,7 +7261,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -7294,7 +7332,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -7365,7 +7403,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -7436,7 +7474,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="39">
         <v>7</v>
       </c>
@@ -7507,7 +7545,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="39">
         <v>7</v>
       </c>
@@ -7578,7 +7616,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="39">
         <v>7</v>
       </c>
@@ -7649,7 +7687,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
       </c>
@@ -7720,7 +7758,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
@@ -7791,7 +7829,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>8</v>
       </c>
@@ -7868,7 +7906,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7879,34 +7917,34 @@
       <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.109375" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -7977,7 +8015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="39">
         <v>1</v>
       </c>
@@ -8048,7 +8086,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8119,7 +8157,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="39">
         <v>3</v>
       </c>
@@ -8190,7 +8228,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -8261,7 +8299,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="39">
         <v>5</v>
       </c>
@@ -8332,7 +8370,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="39">
         <v>5</v>
       </c>
@@ -8403,7 +8441,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="39">
         <v>5</v>
       </c>
@@ -8474,7 +8512,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -8545,7 +8583,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -8616,7 +8654,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -8687,7 +8725,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="39">
         <v>7</v>
       </c>
@@ -8758,7 +8796,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="39">
         <v>7</v>
       </c>
@@ -8829,7 +8867,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="39">
         <v>7</v>
       </c>
@@ -8900,7 +8938,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
       </c>
@@ -8971,7 +9009,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
@@ -9042,7 +9080,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>8</v>
       </c>
@@ -9113,7 +9151,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="39">
         <v>9</v>
       </c>
@@ -9184,7 +9222,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="39">
         <v>9</v>
       </c>
@@ -9255,7 +9293,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10</v>
       </c>
@@ -9326,7 +9364,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>10</v>
       </c>
@@ -9397,7 +9435,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="39">
         <v>11</v>
       </c>
@@ -9468,7 +9506,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="39">
         <v>11</v>
       </c>
@@ -9539,7 +9577,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>12</v>
       </c>
@@ -9610,7 +9648,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>12</v>
       </c>
@@ -9681,7 +9719,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="39">
         <v>13</v>
       </c>
@@ -9752,7 +9790,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="39">
         <v>13</v>
       </c>
@@ -9823,7 +9861,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="39">
         <v>13</v>
       </c>
@@ -9894,7 +9932,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="39">
         <v>13</v>
       </c>
@@ -9965,7 +10003,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="39">
         <v>13</v>
       </c>
@@ -10036,7 +10074,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="39">
         <v>13</v>
       </c>
@@ -10107,7 +10145,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>14</v>
       </c>
@@ -10178,7 +10216,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>14</v>
       </c>
@@ -10249,7 +10287,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>14</v>
       </c>
@@ -10320,7 +10358,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>14</v>
       </c>
@@ -10391,7 +10429,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>14</v>
       </c>
@@ -10462,7 +10500,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>14</v>
       </c>
@@ -10533,7 +10571,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38" s="39">
         <v>15</v>
       </c>
@@ -10604,7 +10642,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" s="39">
         <v>15</v>
       </c>
@@ -10675,7 +10713,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" s="39">
         <v>15</v>
       </c>
@@ -10746,7 +10784,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" s="39">
         <v>15</v>
       </c>
@@ -10817,7 +10855,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" s="39">
         <v>15</v>
       </c>
@@ -10888,7 +10926,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" s="39">
         <v>15</v>
       </c>
@@ -10959,7 +10997,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>16</v>
       </c>
@@ -11030,7 +11068,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>16</v>
       </c>
@@ -11101,7 +11139,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>16</v>
       </c>
@@ -11172,7 +11210,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>16</v>
       </c>
@@ -11243,7 +11281,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>16</v>
       </c>
@@ -11314,7 +11352,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>16</v>
       </c>
@@ -11391,7 +11429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11401,15 +11439,15 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="66.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="66.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>46</v>
       </c>
@@ -11423,7 +11461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>22</v>
       </c>
@@ -11437,7 +11475,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="56" t="s">
         <v>1</v>
       </c>
@@ -11447,9 +11485,9 @@
       <c r="C3" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="68"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="62"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -11461,7 +11499,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -11473,7 +11511,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -11487,7 +11525,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>84</v>
       </c>
@@ -11501,7 +11539,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>85</v>
       </c>
@@ -11512,10 +11550,10 @@
         <v>90</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>86</v>
       </c>
@@ -11529,7 +11567,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="56" t="s">
         <v>129</v>
       </c>
@@ -11539,11 +11577,11 @@
       <c r="C10" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="D10" s="66" t="s">
+      <c r="D10" s="69" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="56" t="s">
         <v>130</v>
       </c>
@@ -11553,9 +11591,9 @@
       <c r="C11" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="D11" s="67"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="70"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="56" t="s">
         <v>136</v>
       </c>
@@ -11569,7 +11607,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="56" t="s">
         <v>137</v>
       </c>
@@ -11583,7 +11621,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="56" t="s">
         <v>138</v>
       </c>
@@ -11597,7 +11635,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="56" t="s">
         <v>139</v>
       </c>
@@ -11611,7 +11649,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="56" t="s">
         <v>140</v>
       </c>
@@ -11625,7 +11663,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="56" t="s">
         <v>141</v>
       </c>
@@ -11639,7 +11677,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="56" t="s">
         <v>142</v>
       </c>
@@ -11653,7 +11691,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="56" t="s">
         <v>143</v>
       </c>
@@ -11667,7 +11705,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="56" t="s">
         <v>144</v>
       </c>
@@ -11681,7 +11719,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="56" t="s">
         <v>145</v>
       </c>
@@ -11695,7 +11733,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="56" t="s">
         <v>146</v>
       </c>
@@ -11709,7 +11747,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="56" t="s">
         <v>147</v>
       </c>
@@ -11723,7 +11761,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="56" t="s">
         <v>127</v>
       </c>
@@ -11735,7 +11773,7 @@
       </c>
       <c r="D24" s="58"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -11747,7 +11785,7 @@
       </c>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
@@ -11761,7 +11799,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="44" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" s="44" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>65</v>
       </c>
@@ -11771,11 +11809,11 @@
       <c r="C27" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="64" t="s">
+      <c r="D27" s="67" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="44" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" s="44" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>64</v>
       </c>
@@ -11785,9 +11823,9 @@
       <c r="C28" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="65"/>
-    </row>
-    <row r="29" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="68"/>
+    </row>
+    <row r="29" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>35</v>
       </c>
@@ -11797,11 +11835,11 @@
       <c r="C29" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="64" t="s">
+      <c r="D29" s="67" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>36</v>
       </c>
@@ -11811,9 +11849,9 @@
       <c r="C30" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D30" s="65"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="68"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="41" t="s">
         <v>13</v>
       </c>
@@ -11827,7 +11865,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>15</v>
       </c>
@@ -11841,7 +11879,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>66</v>
       </c>
@@ -11851,11 +11889,11 @@
       <c r="C33" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="D33" s="64" t="s">
+      <c r="D33" s="67" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>67</v>
       </c>
@@ -11865,9 +11903,9 @@
       <c r="C34" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="65"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="68"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>33</v>
       </c>
@@ -11877,11 +11915,11 @@
       <c r="C35" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="64" t="s">
+      <c r="D35" s="67" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>34</v>
       </c>
@@ -11891,325 +11929,325 @@
       <c r="C36" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="65"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="68"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
     </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
     </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
     </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
     </row>
-    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
     </row>
-    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
     </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
     </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
     </row>
@@ -12227,7 +12265,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AG5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12235,70 +12273,70 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="26" max="27" width="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="12" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:33" s="63" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="63" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="70" t="s">
+      <c r="I1" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="70" t="s">
+      <c r="J1" s="64" t="s">
         <v>130</v>
       </c>
       <c r="K1" s="60" t="s">
@@ -12337,41 +12375,41 @@
       <c r="V1" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="W1" s="70" t="s">
+      <c r="W1" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="X1" s="69" t="s">
+      <c r="X1" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="69" t="s">
+      <c r="Y1" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="69" t="s">
+      <c r="Z1" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="AA1" s="69" t="s">
+      <c r="AA1" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="AB1" s="69" t="s">
+      <c r="AB1" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="AC1" s="69" t="s">
+      <c r="AC1" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="69" t="s">
+      <c r="AD1" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="69" t="s">
+      <c r="AE1" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="AF1" s="69" t="s">
+      <c r="AF1" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="AG1" s="69" t="s">
+      <c r="AG1" s="63" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -12472,7 +12510,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -12573,7 +12611,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -12674,7 +12712,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -12782,7 +12820,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12790,66 +12828,66 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:27" s="63" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="63" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="70" t="s">
+      <c r="I1" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="70" t="s">
+      <c r="J1" s="64" t="s">
         <v>130</v>
       </c>
       <c r="K1" s="60" t="s">
@@ -12888,23 +12926,23 @@
       <c r="V1" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="W1" s="70" t="s">
+      <c r="W1" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="X1" s="69" t="s">
+      <c r="X1" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="69" t="s">
+      <c r="Y1" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="69" t="s">
+      <c r="Z1" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="69" t="s">
+      <c r="AA1" s="63" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -12993,7 +13031,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13001,70 +13039,70 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="12" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:31" s="63" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="63" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="70" t="s">
+      <c r="I1" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="70" t="s">
+      <c r="J1" s="64" t="s">
         <v>130</v>
       </c>
       <c r="K1" s="60" t="s">
@@ -13103,35 +13141,35 @@
       <c r="V1" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="W1" s="70" t="s">
+      <c r="W1" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="X1" s="69" t="s">
+      <c r="X1" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="Y1" s="69" t="s">
+      <c r="Y1" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="69" t="s">
+      <c r="Z1" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="AA1" s="69" t="s">
+      <c r="AA1" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="AB1" s="69" t="s">
+      <c r="AB1" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="69" t="s">
+      <c r="AC1" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="AD1" s="69" t="s">
+      <c r="AD1" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="AE1" s="69" t="s">
+      <c r="AE1" s="63" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -13226,7 +13264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -13321,7 +13359,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -13416,7 +13454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>

</xml_diff>